<commit_message>
Modificacion de algunos archivos basModificacion de arhivos
</commit_message>
<xml_diff>
--- a/bin/Formatos/Extracto.xlsx
+++ b/bin/Formatos/Extracto.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\Transacciones_davivienda\src\Plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\auto_javarturs\src\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56CE02E-0F65-4BD3-AA9D-FF6D09FA00AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB39703A-B174-4236-A75D-3619A17FDA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="810" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AGROPECUARIA SANTA MARIA" sheetId="78" r:id="rId1"/>
+    <sheet name="PLANTILLA" sheetId="78" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'AGROPECUARIA SANTA MARIA'!$A$1:$G$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PLANTILLA!$A$1:$G$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -146,42 +146,6 @@
     <t xml:space="preserve">RESPONSABLE DEL CONTRATANTE </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">CONVENIO CONSORCIO UNION TEMPORAL CON:                                                </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> NIT:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">NIT: </t>
   </si>
   <si>
@@ -225,6 +189,9 @@
   </si>
   <si>
     <t>C-AAAA</t>
+  </si>
+  <si>
+    <t>CONVENIO CONSORCIO UNION TEMPORAL CON:</t>
   </si>
 </sst>
 </file>
@@ -651,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -734,44 +701,65 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -779,6 +767,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -809,119 +860,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1476,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,31 +1469,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
+      <c r="A1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="89"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="91"/>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
@@ -1538,156 +1514,156 @@
       <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="A6" s="87" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="74"/>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+      <c r="A9" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="80"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53" t="s">
+      <c r="D11" s="58"/>
+      <c r="E11" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="56"/>
+      <c r="A12" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="61"/>
       <c r="C12" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="53" t="s">
+    <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="62"/>
+      <c r="E13" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
-    </row>
-    <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="64"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
+    </row>
+    <row r="16" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="62"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="70"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="42"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
         <v>3</v>
@@ -1695,10 +1671,10 @@
       <c r="E18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="67"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
@@ -1708,29 +1684,29 @@
         <v>0</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="89">
+        <v>41</v>
+      </c>
+      <c r="F19" s="28">
         <v>0</v>
       </c>
-      <c r="G19" s="90"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="66" t="s">
+      <c r="F20" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="67"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -1740,239 +1716,239 @@
         <v>0</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="89">
+        <v>41</v>
+      </c>
+      <c r="F21" s="28">
         <v>0</v>
       </c>
-      <c r="G21" s="90"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="65"/>
+      <c r="A22" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="73" t="s">
+      <c r="B23" s="52"/>
+      <c r="C23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="72"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="73" t="s">
+      <c r="F23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="65"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="76">
+      <c r="A24" s="53"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="34">
         <v>2006</v>
       </c>
-      <c r="D24" s="75"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="78"/>
+        <v>39</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="73" t="s">
+      <c r="B25" s="51"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="65"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="74">
+      <c r="A26" s="53">
         <v>2019</v>
       </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76">
+      <c r="B26" s="55"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="34">
         <v>336392</v>
       </c>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="69"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="66" t="s">
+      <c r="F27" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="67"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
-      <c r="B28" s="71"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="26"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="80"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="69"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="66" t="s">
+      <c r="F29" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="67"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="70"/>
-      <c r="B30" s="71"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="26"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="82"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="69"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="66" t="s">
+      <c r="F31" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="67"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
-      <c r="B32" s="71"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="26"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="80"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="69"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="66" t="s">
+      <c r="F33" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="67"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="85"/>
-      <c r="B34" s="86"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="88"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="45"/>
     </row>
     <row r="35" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
+      <c r="A37" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="84" t="s">
+      <c r="A38" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="84"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
     </row>
     <row r="39" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="84" t="s">
+      <c r="A39" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="84"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="84"/>
-      <c r="F39" s="84"/>
-      <c r="G39" s="84"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
     </row>
     <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="84" t="s">
+      <c r="A40" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="84"/>
-      <c r="G40" s="84"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -2003,21 +1979,30 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="A33:B34"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="A29:B30"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:G22"/>
@@ -2034,30 +2019,21 @@
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.78740157480314965"/>

</xml_diff>

<commit_message>
Cambios en diferentes clases para el funcionamiento correcto de insercion de extractos mensuales junto con el cambio de los metodos respectivos
</commit_message>
<xml_diff>
--- a/bin/Formatos/Extracto.xlsx
+++ b/bin/Formatos/Extracto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\auto_javarturs\src\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB39703A-B174-4236-A75D-3619A17FDA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886A1628-94FA-4044-B65A-D2CE6671FDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA" sheetId="78" r:id="rId1"/>
@@ -701,65 +701,44 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -767,28 +746,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -830,74 +815,89 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,31 +1469,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81"/>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="89"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="91"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="85"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
@@ -1514,78 +1514,78 @@
       <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="77"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="80"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="71"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="61"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="22" t="s">
         <v>43</v>
       </c>
@@ -1595,14 +1595,14 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="62" t="s">
+      <c r="B13" s="56"/>
+      <c r="C13" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="62"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1610,60 +1610,60 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="63" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
-    </row>
-    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+    </row>
+    <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="65" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
     </row>
     <row r="16" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="61" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="61"/>
-      <c r="G16" s="70"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="33"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
         <v>3</v>
@@ -1671,10 +1671,10 @@
       <c r="E18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="70"/>
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
@@ -1686,27 +1686,27 @@
       <c r="E19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="92">
         <v>0</v>
       </c>
-      <c r="G19" s="29"/>
+      <c r="G19" s="93"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="70"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -1718,85 +1718,85 @@
       <c r="E21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="92">
         <v>0</v>
       </c>
-      <c r="G21" s="29"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="33"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="68"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="32" t="s">
+      <c r="B23" s="75"/>
+      <c r="C23" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="33"/>
+      <c r="G23" s="68"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="34">
+      <c r="A24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79">
         <v>2006</v>
       </c>
-      <c r="D24" s="54"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="35"/>
+      <c r="G24" s="81"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="32" t="s">
+      <c r="B25" s="67"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="33"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="53">
+      <c r="A26" s="77">
         <v>2019</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="34">
+      <c r="B26" s="80"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="79">
         <v>336392</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="35"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="81"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="39"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="10" t="s">
         <v>12</v>
       </c>
@@ -1806,25 +1806,25 @@
       <c r="E27" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="31"/>
+      <c r="G27" s="70"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="26"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="39"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="18" t="s">
         <v>12</v>
       </c>
@@ -1834,25 +1834,25 @@
       <c r="E29" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="31"/>
+      <c r="G29" s="70"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="26"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="57"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="39"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
@@ -1862,25 +1862,25 @@
       <c r="E31" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="31"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="26"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="83"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="12" t="s">
         <v>12</v>
       </c>
@@ -1890,65 +1890,65 @@
       <c r="E33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="70"/>
     </row>
     <row r="34" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="91"/>
     </row>
     <row r="35" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
     </row>
     <row r="38" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
     </row>
     <row r="39" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
     </row>
     <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -1979,30 +1979,21 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="A29:B30"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:G22"/>
@@ -2019,21 +2010,30 @@
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="A33:B34"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.78740157480314965"/>

</xml_diff>

<commit_message>
MOdificacion de las clases extractos, sobre que no se exactamente, sin embargo supongo que es para exportar de una mejor manera
</commit_message>
<xml_diff>
--- a/bin/Formatos/Extracto.xlsx
+++ b/bin/Formatos/Extracto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\auto_javarturs\src\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Beltran\Desktop\auto_javarturs\src\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886A1628-94FA-4044-B65A-D2CE6671FDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC227E0E-BBF2-48BC-B6BD-C2C4B6BCA0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA" sheetId="78" r:id="rId1"/>
@@ -674,9 +674,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,44 +698,65 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -746,6 +764,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -776,128 +857,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,124 +1469,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="88"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="90"/>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="92"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="23"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="23"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="79"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="70"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53" t="s">
+      <c r="D11" s="57"/>
+      <c r="E11" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="3"/>
@@ -1595,14 +1595,14 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="57" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="57"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1610,60 +1610,60 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="58" t="s">
+      <c r="B14" s="60"/>
+      <c r="C14" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="63"/>
     </row>
     <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="60" t="s">
+      <c r="B15" s="60"/>
+      <c r="C15" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="66"/>
     </row>
     <row r="16" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="56" t="s">
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="65"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="69"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="68"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="42"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
         <v>3</v>
@@ -1671,10 +1671,10 @@
       <c r="E18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="69" t="s">
+      <c r="F18" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="70"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
@@ -1686,27 +1686,27 @@
       <c r="E19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="92">
+      <c r="F19" s="27">
         <v>0</v>
       </c>
-      <c r="G19" s="93"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="69" t="s">
+      <c r="F20" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="70"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -1718,169 +1718,169 @@
       <c r="E21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="92">
+      <c r="F21" s="27">
         <v>0</v>
       </c>
-      <c r="G21" s="93"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="68"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="76" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="75"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="76" t="s">
+      <c r="F23" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="68"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
-      <c r="B24" s="78"/>
-      <c r="C24" s="79">
+      <c r="A24" s="52"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="33">
         <v>2006</v>
       </c>
-      <c r="D24" s="78"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="79" t="s">
+      <c r="F24" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="81"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="76" t="s">
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="68"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="77">
+      <c r="A26" s="52">
         <v>2019</v>
       </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="79">
+      <c r="B26" s="54"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="33">
         <v>336392</v>
       </c>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="81"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="72"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="69" t="s">
+      <c r="F27" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="70"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="46"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="72"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="69" t="s">
+      <c r="F29" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="70"/>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="85"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="56"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="72"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="69" t="s">
+      <c r="F31" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="70"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="83"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="46"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="72"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="12" t="s">
         <v>12</v>
       </c>
@@ -1890,65 +1890,65 @@
       <c r="E33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="69" t="s">
+      <c r="F33" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="70"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="88"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="90"/>
-      <c r="G34" s="91"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
     </row>
     <row r="35" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="86" t="s">
+      <c r="A37" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="87"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="87"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="87" t="s">
+      <c r="A40" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="87"/>
-      <c r="C40" s="87"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -1979,21 +1979,30 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="A33:B34"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="A29:B30"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:G22"/>
@@ -2010,30 +2019,21 @@
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.78740157480314965"/>

</xml_diff>

<commit_message>
Modificacion de ciertos archivos para evitar errores de memoria durante la compilacion
</commit_message>
<xml_diff>
--- a/bin/Formatos/Extracto.xlsx
+++ b/bin/Formatos/Extracto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Beltran\Desktop\auto_javarturs\src\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\auto_javarturs\src\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC227E0E-BBF2-48BC-B6BD-C2C4B6BCA0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1BFB5E-5AD8-4644-8079-9042EEF5F0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA" sheetId="78" r:id="rId1"/>
@@ -698,65 +698,47 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -764,28 +746,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -827,77 +815,89 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,8 +1145,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>65288</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>48453</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>153228</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,31 +1469,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80"/>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="88"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="90"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="84"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="92"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
@@ -1514,78 +1514,78 @@
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="73"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="76"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="79"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="70"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="60"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="21" t="s">
         <v>43</v>
       </c>
@@ -1595,14 +1595,14 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="61" t="s">
+      <c r="B13" s="56"/>
+      <c r="C13" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="61"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1610,60 +1610,60 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="62" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="63"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
     </row>
     <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="64" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="66"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
     </row>
     <row r="16" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="60" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="69"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="32"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="48"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
         <v>3</v>
@@ -1671,10 +1671,10 @@
       <c r="E18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="70"/>
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
@@ -1686,27 +1686,27 @@
       <c r="E19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="92">
         <v>0</v>
       </c>
-      <c r="G19" s="28"/>
+      <c r="G19" s="93"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="70"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -1718,85 +1718,85 @@
       <c r="E21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="92">
         <v>0</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="32"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="68"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="31" t="s">
+      <c r="B23" s="75"/>
+      <c r="C23" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="51"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="68"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="33">
+      <c r="A24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79">
         <v>2006</v>
       </c>
-      <c r="D24" s="53"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="34"/>
+      <c r="G24" s="81"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="31" t="s">
+      <c r="B25" s="67"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="32"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
+      <c r="A26" s="77">
         <v>2019</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="33">
+      <c r="B26" s="80"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="79">
         <v>336392</v>
       </c>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="34"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="81"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="10" t="s">
         <v>12</v>
       </c>
@@ -1806,25 +1806,25 @@
       <c r="E27" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="70"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="B28" s="40"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="25"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="18" t="s">
         <v>12</v>
       </c>
@@ -1834,25 +1834,25 @@
       <c r="E29" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="30"/>
+      <c r="G29" s="70"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="56"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
@@ -1862,25 +1862,25 @@
       <c r="E31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="25"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="46"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="83"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="12" t="s">
         <v>12</v>
       </c>
@@ -1890,65 +1890,65 @@
       <c r="E33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="F33" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="41"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="93"/>
+      <c r="G33" s="70"/>
+    </row>
+    <row r="34" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="88"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="19"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="91"/>
     </row>
     <row r="35" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
     </row>
     <row r="38" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
     </row>
     <row r="39" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
     </row>
     <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -1979,30 +1979,21 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="A29:B30"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:G22"/>
@@ -2019,21 +2010,30 @@
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="A33:B34"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.78740157480314965"/>

</xml_diff>

<commit_message>
Modificacino completa de la base de datos
</commit_message>
<xml_diff>
--- a/bin/Formatos/Extracto.xlsx
+++ b/bin/Formatos/Extracto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\auto_javarturs\src\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\auto_javarturs\src\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8615A8D-EA06-4020-9295-765EEC390CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF7CDA8-8165-4CE8-9420-92C53837A1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5505" yWindow="2835" windowWidth="19410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA" sheetId="78" r:id="rId1"/>
@@ -701,65 +701,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -767,28 +746,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -830,74 +815,89 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1031,59 +1031,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="4 Imagen" descr="Descripción: D:\usuario\Documents\logovigilados,.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4191000" y="1066800"/>
-          <a:ext cx="1771651" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
       <xdr:row>34</xdr:row>
@@ -1107,7 +1054,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1162,7 +1109,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1176,6 +1123,50 @@
         <a:xfrm>
           <a:off x="3409950" y="7572375"/>
           <a:ext cx="1684538" cy="1743903"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>612323</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>743843</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>352686</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E0EAB7-2BCB-DC2A-B2BC-09E56E016CD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4212773" y="1019175"/>
+          <a:ext cx="1960320" cy="571761"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1452,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,31 +1460,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81"/>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="89"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="91"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="85"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
@@ -1514,78 +1505,78 @@
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="77"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="80"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="71"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="61"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="21" t="s">
         <v>43</v>
       </c>
@@ -1595,14 +1586,14 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="62" t="s">
+      <c r="B13" s="56"/>
+      <c r="C13" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="62"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1610,60 +1601,60 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="63" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
     </row>
     <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="65" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
     </row>
     <row r="16" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="61" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="61"/>
-      <c r="G16" s="70"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="33"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
         <v>3</v>
@@ -1671,10 +1662,10 @@
       <c r="E18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="70"/>
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
@@ -1686,27 +1677,27 @@
       <c r="E19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="92">
         <v>0</v>
       </c>
-      <c r="G19" s="29"/>
+      <c r="G19" s="93"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="70"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -1718,85 +1709,85 @@
       <c r="E21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="92">
         <v>0</v>
       </c>
-      <c r="G21" s="29"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="33"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="68"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="32" t="s">
+      <c r="B23" s="75"/>
+      <c r="C23" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="33"/>
+      <c r="G23" s="68"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="34">
+      <c r="A24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79">
         <v>2006</v>
       </c>
-      <c r="D24" s="54"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="35"/>
+      <c r="G24" s="81"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="32" t="s">
+      <c r="B25" s="67"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="33"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="53">
+      <c r="A26" s="77">
         <v>2019</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="34">
+      <c r="B26" s="80"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="79">
         <v>336392</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="35"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="81"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="39"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="10" t="s">
         <v>12</v>
       </c>
@@ -1806,25 +1797,25 @@
       <c r="E27" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="31"/>
+      <c r="G27" s="70"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="25"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="39"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="18" t="s">
         <v>12</v>
       </c>
@@ -1834,25 +1825,25 @@
       <c r="E29" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="31"/>
+      <c r="G29" s="70"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="57"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="39"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
@@ -1862,25 +1853,25 @@
       <c r="E31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="31"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="25"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="83"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="12" t="s">
         <v>12</v>
       </c>
@@ -1890,65 +1881,65 @@
       <c r="E33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="70"/>
     </row>
     <row r="34" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="27"/>
       <c r="D34" s="19"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="91"/>
     </row>
     <row r="35" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
     </row>
     <row r="38" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
     </row>
     <row r="39" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
     </row>
     <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -1979,30 +1970,21 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="A29:B30"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:G22"/>
@@ -2019,21 +2001,30 @@
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="A33:B34"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.78740157480314965"/>

</xml_diff>